<commit_message>
MP4 V5.1 Data update - Key 인식 오류 개선
</commit_message>
<xml_diff>
--- a/0_MP4 Data/Pipette Change list MP4.xlsx
+++ b/0_MP4 Data/Pipette Change list MP4.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="111">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -436,6 +436,30 @@
   </si>
   <si>
     <t>Femto Science Inc. silk 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Noise로 인한 Key 인식 오류 개선</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1uF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R18,R27,R36</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1425,7 +1449,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1624,6 +1648,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3017,7 +3047,7 @@
   <dimension ref="B1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3145,25 +3175,43 @@
       <c r="B7" s="66">
         <v>5</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="70"/>
+      <c r="C7" s="89">
+        <v>43626</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="71">
+        <v>0</v>
+      </c>
+      <c r="G7" s="69">
+        <v>100</v>
+      </c>
       <c r="H7" s="71"/>
-      <c r="I7" s="72"/>
+      <c r="I7" s="92" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="66">
         <v>6</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="69" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="69" t="s">
+        <v>109</v>
+      </c>
       <c r="H8" s="71"/>
-      <c r="I8" s="72"/>
+      <c r="I8" s="93"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="66">
@@ -3398,8 +3446,11 @@
       <c r="I28" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3453,7 +3504,7 @@
       <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="92">
+      <c r="C3" s="94">
         <v>43460</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -3468,7 +3519,7 @@
       <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="95" t="s">
+      <c r="H3" s="97" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3476,7 +3527,7 @@
       <c r="B4" s="12">
         <v>2</v>
       </c>
-      <c r="C4" s="93"/>
+      <c r="C4" s="95"/>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
@@ -3489,13 +3540,13 @@
       <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="96"/>
+      <c r="H4" s="98"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>3</v>
       </c>
-      <c r="C5" s="93"/>
+      <c r="C5" s="95"/>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3508,13 +3559,13 @@
       <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="96"/>
+      <c r="H5" s="98"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="12">
         <v>4</v>
       </c>
-      <c r="C6" s="93"/>
+      <c r="C6" s="95"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -3527,13 +3578,13 @@
       <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="97"/>
+      <c r="H6" s="99"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>5</v>
       </c>
-      <c r="C7" s="93"/>
+      <c r="C7" s="95"/>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
@@ -3552,7 +3603,7 @@
       <c r="B8" s="12">
         <v>6</v>
       </c>
-      <c r="C8" s="94"/>
+      <c r="C8" s="96"/>
       <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
@@ -3571,7 +3622,7 @@
       <c r="B9" s="12">
         <v>7</v>
       </c>
-      <c r="C9" s="98">
+      <c r="C9" s="100">
         <v>43530</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -3588,7 +3639,7 @@
       <c r="B10" s="12">
         <v>8</v>
       </c>
-      <c r="C10" s="94"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>